<commit_message>
add test results 03/12/25
</commit_message>
<xml_diff>
--- a/spc/results/t01/M_0.20_k_0.05/omp_CLEAN/omp_residuals_run_1.xlsx
+++ b/spc/results/t01/M_0.20_k_0.05/omp_CLEAN/omp_residuals_run_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A205"/>
+  <dimension ref="A1:A92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -895,571 +895,6 @@
         <v>139.5015118531425</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>138.0526917968137</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>136.7546704532724</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>135.393509938787</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>134.0233309646777</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>132.6014562231589</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>131.0904664545839</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>130.0145994824875</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>128.9443230339056</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>127.5702950880335</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>126.3211453843494</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>125.240732773904</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>124.1866289262452</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>123.0620707655233</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>121.8443477855604</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>120.9111493009556</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>119.9296693573994</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>118.9239822471932</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>117.9111835879189</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>116.7161509516335</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>115.5333231455543</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>114.4223440127887</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>113.0983970766081</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n">
-        <v>112.0117301298656</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="n">
-        <v>111.0477819452008</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="n">
-        <v>110.0795414888919</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="n">
-        <v>109.1356330326894</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="n">
-        <v>108.3491173054355</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="n">
-        <v>107.5134905239313</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="n">
-        <v>106.5228174505168</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>105.5232514344395</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n">
-        <v>104.5615800585719</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="n">
-        <v>103.5021625100478</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="n">
-        <v>102.6788144083062</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="n">
-        <v>101.7459209639716</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="n">
-        <v>100.8316023735499</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="n">
-        <v>99.92323252336091</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="n">
-        <v>99.09658741468292</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="n">
-        <v>98.19648445266749</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="n">
-        <v>97.40852246920542</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="n">
-        <v>96.61821734714896</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="n">
-        <v>95.77975562062386</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="n">
-        <v>94.98203583698044</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="n">
-        <v>94.16830881374032</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="n">
-        <v>93.35296778988133</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="n">
-        <v>92.51861745785151</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="n">
-        <v>91.73054356983016</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="n">
-        <v>90.84256204271483</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="n">
-        <v>90.02435213757218</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="n">
-        <v>89.27801402968943</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="n">
-        <v>88.34021649222676</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="n">
-        <v>87.55560810978662</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="n">
-        <v>86.79411397185746</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="n">
-        <v>86.0318375520026</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="n">
-        <v>85.23016992224862</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="n">
-        <v>84.51368402421237</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="n">
-        <v>83.93815345505902</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="n">
-        <v>83.33677342751352</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="n">
-        <v>82.6020859304155</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="n">
-        <v>81.99415544661926</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="n">
-        <v>81.26812324615517</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="n">
-        <v>80.52987009947348</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="n">
-        <v>79.9336795963796</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="n">
-        <v>79.19613336909769</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="n">
-        <v>78.52289483432372</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="n">
-        <v>77.92705395303936</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="n">
-        <v>77.20580193666569</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="n">
-        <v>76.55628426051028</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="n">
-        <v>75.87705712777867</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="n">
-        <v>75.17458825299161</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="n">
-        <v>74.5601786800262</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="n">
-        <v>74.02915461648951</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="n">
-        <v>73.47174799361876</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="n">
-        <v>72.84202951935829</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="n">
-        <v>72.30467272041285</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="n">
-        <v>71.75650467889324</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="n">
-        <v>71.24112940303418</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="n">
-        <v>70.75616674326</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="n">
-        <v>70.26317503560331</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="n">
-        <v>69.81236473863184</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="n">
-        <v>69.34455636240182</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="n">
-        <v>68.89583593221535</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="n">
-        <v>68.49720797779887</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="n">
-        <v>68.03365662640172</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="n">
-        <v>67.55659065397808</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="n">
-        <v>67.1227861609606</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="n">
-        <v>66.67870420935479</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="n">
-        <v>66.17769590123025</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="n">
-        <v>65.71584610904544</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="n">
-        <v>65.27203859003207</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="n">
-        <v>64.86380007193388</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="n">
-        <v>64.42783577868852</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="n">
-        <v>63.95056897202308</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="n">
-        <v>63.49977472329493</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="n">
-        <v>63.07047894734045</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="n">
-        <v>62.64064097810428</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="n">
-        <v>62.20549617567992</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="n">
-        <v>61.73439456409059</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="n">
-        <v>61.35742992407334</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="n">
-        <v>60.91235109582823</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="n">
-        <v>60.45508709237301</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="n">
-        <v>59.98648453900523</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="n">
-        <v>59.64101760869085</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="n">
-        <v>59.26693365743657</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="n">
-        <v>58.85959146509528</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="n">
-        <v>58.43762289385587</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="n">
-        <v>58.04024829960167</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="n">
-        <v>57.60184544289341</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="n">
-        <v>57.21355916793033</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="n">
-        <v>56.74524857290544</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="n">
-        <v>56.28769113774246</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="n">
-        <v>55.9007712577868</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="n">
-        <v>55.53263651086691</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="n">
-        <v>55.15280697110039</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>